<commit_message>
Updated human evaluation tabular
</commit_message>
<xml_diff>
--- a/Human_Evaluation.xlsx
+++ b/Human_Evaluation.xlsx
@@ -1,62 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabe\OneDrive\Dokumente\NLP vaje 2\ul-fri-nlp-course-project-2024-2025-the-parse-force\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2CA1DF-0EAE-41E2-82C1-A510E1FDCBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Sentence ID</t>
   </si>
   <si>
-    <t>Language Pair (ENG-GER, GER-SLO, ENG-SLO)</t>
-  </si>
-  <si>
     <t>Original Source Sentence</t>
   </si>
   <si>
     <t>Machine Translation Output</t>
   </si>
   <si>
-    <t>Reference Human Translation</t>
-  </si>
-  <si>
-    <t>Formality Rating (-3 to +3)</t>
-  </si>
-  <si>
-    <t>Formality Comment (optional)</t>
-  </si>
-  <si>
-    <t>Fluency Rating (1-5)</t>
-  </si>
-  <si>
-    <t>Fluency Comment (optional)</t>
-  </si>
-  <si>
-    <t>Meaning Preservation Rating (1-6)</t>
-  </si>
-  <si>
-    <t>Meaning Preservation Comment (optional)</t>
-  </si>
-  <si>
-    <t>Additional Comments (optional)</t>
+    <r>
+      <t>Language Pair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(ENG-GER, GER-SLO, ENG-SLO)</t>
+    </r>
+  </si>
+  <si>
+    <t>Formality Rating
+ (-3 to +3)</t>
+  </si>
+  <si>
+    <t>Formality Comment
+ (optional)</t>
+  </si>
+  <si>
+    <t>Fluency Rating 
+(1-5)</t>
+  </si>
+  <si>
+    <t>Fluency Comment
+ (optional)</t>
+  </si>
+  <si>
+    <t>Meaning Preservation Rating 
+(1-6)</t>
+  </si>
+  <si>
+    <t>Meaning Preservation 
+Comment (optional)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,12 +92,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -108,24 +151,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +226,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -197,6 +260,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -231,9 +295,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,49 +471,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="30.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.7265625" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="23.08984375" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.54296875" customWidth="1"/>
+    <col min="10" max="10" width="26.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>